<commit_message>
Cambios en jueves 16 y viernes 17 por compromiso
</commit_message>
<xml_diff>
--- a/Programacion de Actividades.xlsx
+++ b/Programacion de Actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1626166-DB5C-4FDD-A022-73E158B14496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B597BB3-0F3B-43E8-A1F0-0A111F6FE661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -399,142 +399,142 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -846,34 +846,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -936,94 +936,94 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="48"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="28" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="33" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="4"/>
       <c r="F6" s="11" t="s">
         <v>17</v>
@@ -1033,129 +1033,129 @@
         <v>18</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="13" t="s">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="21" t="s">
+      <c r="M6" s="14"/>
+      <c r="N6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="22" t="s">
+      <c r="O6" s="15"/>
+      <c r="P6" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="45" t="s">
+      <c r="G8" s="28"/>
+      <c r="H8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="13" t="s">
+      <c r="I8" s="29"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="13"/>
-      <c r="N8" s="21" t="s">
+      <c r="M8" s="14"/>
+      <c r="N8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="42" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
       <c r="K9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="13" t="s">
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
         <v>18</v>
@@ -1163,89 +1163,89 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="21" t="s">
+      <c r="J10" s="47"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="13" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="28" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="9" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="5"/>
       <c r="F13" s="11" t="s">
         <v>17</v>
@@ -1255,61 +1255,61 @@
         <v>18</v>
       </c>
       <c r="I13" s="12"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="13" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="21" t="s">
+      <c r="M13" s="14"/>
+      <c r="N13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="25" t="s">
+      <c r="O13" s="15"/>
+      <c r="P13" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="9" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="5"/>
       <c r="F15" s="11" t="s">
         <v>17</v>
@@ -1319,219 +1319,219 @@
         <v>18</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="13" t="s">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="21" t="s">
+      <c r="M15" s="14"/>
+      <c r="N15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="21"/>
-      <c r="P15" s="28" t="s">
+      <c r="O15" s="15"/>
+      <c r="P15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="13" t="s">
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="5"/>
       <c r="F17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="21" t="s">
+      <c r="I17" s="35"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="32" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="13" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="28" t="s">
+      <c r="H18" s="14"/>
+      <c r="I18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="34" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="4"/>
       <c r="F20" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="20" t="s">
+      <c r="I20" s="39"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="39" t="s">
+      <c r="M20" s="48"/>
+      <c r="N20" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="39"/>
-      <c r="P20" s="28" t="s">
+      <c r="O20" s="38"/>
+      <c r="P20" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="24" t="s">
+      <c r="D21" s="25"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="5"/>
       <c r="F22" s="11" t="s">
         <v>17</v>
@@ -1541,155 +1541,155 @@
         <v>18</v>
       </c>
       <c r="I22" s="12"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="40" t="s">
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="40"/>
-      <c r="N22" s="21" t="s">
+      <c r="M22" s="45"/>
+      <c r="N22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="28" t="s">
+      <c r="O22" s="15"/>
+      <c r="P22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="24"/>
       <c r="K23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
-      <c r="N23" s="35" t="s">
+      <c r="N23" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="36"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="13" t="s">
+      <c r="O23" s="42"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="5"/>
       <c r="F24" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="39" t="s">
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="39"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="32" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="13" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="28" t="s">
+      <c r="H25" s="14"/>
+      <c r="I25" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="31" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="5"/>
       <c r="F27" s="11" t="s">
         <v>17</v>
@@ -1699,61 +1699,61 @@
         <v>18</v>
       </c>
       <c r="I27" s="12"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="13" t="s">
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="21" t="s">
+      <c r="M27" s="14"/>
+      <c r="N27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="21"/>
-      <c r="P27" s="22" t="s">
+      <c r="O27" s="15"/>
+      <c r="P27" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="33" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="5"/>
       <c r="F29" s="11" t="s">
         <v>17</v>
@@ -1763,65 +1763,65 @@
         <v>18</v>
       </c>
       <c r="I29" s="12"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M29" s="13"/>
-      <c r="N29" s="21" t="s">
+      <c r="M29" s="14"/>
+      <c r="N29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O29" s="21"/>
-      <c r="P29" s="28" t="s">
+      <c r="O29" s="15"/>
+      <c r="P29" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="13" t="s">
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="5"/>
       <c r="F31" s="12" t="s">
         <v>30</v>
@@ -1829,49 +1829,126 @@
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="21" t="s">
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="155">
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="E5:O5"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:O7"/>
-    <mergeCell ref="K4:T4"/>
-    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="Q31:T31"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="Q17:T17"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="E14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:T25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:O26"/>
+    <mergeCell ref="P26:T26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:O28"/>
+    <mergeCell ref="P28:T28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:T18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:O19"/>
+    <mergeCell ref="P19:T19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="P21:T21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
@@ -1896,110 +1973,33 @@
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:T18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:O19"/>
-    <mergeCell ref="P19:T19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="L24:P24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="P21:T21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:T25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:O26"/>
-    <mergeCell ref="P26:T26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="E14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="Q31:T31"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="Q17:T17"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:O7"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="E5:O5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Domingo 19, debo programar todo el día para poder cumplir con el laboratorio 1
</commit_message>
<xml_diff>
--- a/Programacion de Actividades.xlsx
+++ b/Programacion de Actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B597BB3-0F3B-43E8-A1F0-0A111F6FE661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB1DB80-C770-4D88-A4B9-0F1F183FDB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="33">
   <si>
     <t>Hora</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>6 al 10</t>
+  </si>
+  <si>
+    <t>Ejercicios Lab 1 Informática</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,19 +402,19 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -420,121 +423,124 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="135"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -819,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:O8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,34 +852,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="51"/>
       <c r="C2" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -936,94 +942,94 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="8"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="48"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="14" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="20" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="21" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="4"/>
       <c r="F6" s="11" t="s">
         <v>17</v>
@@ -1033,129 +1039,129 @@
         <v>18</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="14" t="s">
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15" t="s">
+      <c r="M6" s="13"/>
+      <c r="N6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="31" t="s">
+      <c r="O6" s="21"/>
+      <c r="P6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="22" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29" t="s">
+      <c r="G8" s="44"/>
+      <c r="H8" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="14" t="s">
+      <c r="I8" s="45"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15" t="s">
+      <c r="M8" s="13"/>
+      <c r="N8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="36" t="s">
+      <c r="O8" s="21"/>
+      <c r="P8" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="34" t="s">
+      <c r="N9" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="14" t="s">
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
         <v>18</v>
@@ -1163,89 +1169,91 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="15" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="14" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="20" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="22" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="5"/>
       <c r="F13" s="11" t="s">
         <v>17</v>
@@ -1255,61 +1263,61 @@
         <v>18</v>
       </c>
       <c r="I13" s="12"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="14" t="s">
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15" t="s">
+      <c r="M13" s="13"/>
+      <c r="N13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="50" t="s">
+      <c r="O13" s="21"/>
+      <c r="P13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="22" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="44"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="5"/>
       <c r="F15" s="11" t="s">
         <v>17</v>
@@ -1319,219 +1327,219 @@
         <v>18</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="14" t="s">
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15" t="s">
+      <c r="M15" s="13"/>
+      <c r="N15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="20" t="s">
+      <c r="O15" s="21"/>
+      <c r="P15" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="24"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="14" t="s">
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="5"/>
       <c r="F17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="15" t="s">
+      <c r="I17" s="38"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
     </row>
     <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="14" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="20" t="s">
+      <c r="H18" s="13"/>
+      <c r="I18" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="40" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="4"/>
       <c r="F20" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="39" t="s">
+      <c r="H20" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="48" t="s">
+      <c r="I20" s="41"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="48"/>
-      <c r="N20" s="38" t="s">
+      <c r="M20" s="20"/>
+      <c r="N20" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="38"/>
-      <c r="P20" s="20" t="s">
+      <c r="O20" s="39"/>
+      <c r="P20" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="44" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="5"/>
       <c r="F22" s="11" t="s">
         <v>17</v>
@@ -1541,155 +1549,155 @@
         <v>18</v>
       </c>
       <c r="I22" s="12"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="45" t="s">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="45"/>
-      <c r="N22" s="15" t="s">
+      <c r="M22" s="40"/>
+      <c r="N22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="20" t="s">
+      <c r="O22" s="21"/>
+      <c r="P22" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="24"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="17"/>
       <c r="K23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
-      <c r="N23" s="41" t="s">
+      <c r="N23" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="42"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="14" t="s">
+      <c r="O23" s="36"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="5"/>
       <c r="F24" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="38" t="s">
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="38"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="27" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="14" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="20" t="s">
+      <c r="H25" s="13"/>
+      <c r="I25" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="46" t="s">
+      <c r="D26" s="6"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="25"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="5"/>
       <c r="F27" s="11" t="s">
         <v>17</v>
@@ -1699,61 +1707,61 @@
         <v>18</v>
       </c>
       <c r="I27" s="12"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="14" t="s">
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15" t="s">
+      <c r="M27" s="13"/>
+      <c r="N27" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="15"/>
-      <c r="P27" s="31" t="s">
+      <c r="O27" s="21"/>
+      <c r="P27" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="21" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="27"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="5"/>
       <c r="F29" s="11" t="s">
         <v>17</v>
@@ -1763,65 +1771,65 @@
         <v>18</v>
       </c>
       <c r="I29" s="12"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="14" t="s">
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15" t="s">
+      <c r="M29" s="13"/>
+      <c r="N29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O29" s="15"/>
-      <c r="P29" s="20" t="s">
+      <c r="O29" s="21"/>
+      <c r="P29" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
       <c r="K30" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
-      <c r="N30" s="34" t="s">
+      <c r="N30" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="14" t="s">
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="5"/>
       <c r="F31" s="12" t="s">
         <v>30</v>
@@ -1829,22 +1837,153 @@
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="15" t="s">
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="155">
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="E5:O5"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:O7"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:T11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:O12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P7:T7"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:T18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:O19"/>
+    <mergeCell ref="P19:T19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="P21:T21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:T25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:O26"/>
+    <mergeCell ref="P26:T26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:O28"/>
+    <mergeCell ref="P28:T28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="E14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R22:T22"/>
@@ -1869,137 +2008,6 @@
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="E14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:T25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:O26"/>
-    <mergeCell ref="P26:T26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:T18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:O19"/>
-    <mergeCell ref="P19:T19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="L24:P24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="P21:T21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:T11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:O12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P7:T7"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:O7"/>
-    <mergeCell ref="K4:T4"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="E5:O5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios en viernes 4, sabado 5 y domingo 6 por motivo de parciales
</commit_message>
<xml_diff>
--- a/Programacion de Actividades.xlsx
+++ b/Programacion de Actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB1DB80-C770-4D88-A4B9-0F1F183FDB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB45897-1960-4643-8560-2E5F6F0FC723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="35">
   <si>
     <t>Hora</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>Ejercicios Lab 1 Informática</t>
+  </si>
+  <si>
+    <t>Estudiar para parciales</t>
+  </si>
+  <si>
+    <t>Debo estudiar para parciales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +166,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +253,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -391,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,145 +421,154 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -825,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:T11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,34 +880,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -942,94 +970,94 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="48"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="28" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="33" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="4"/>
       <c r="F6" s="11" t="s">
         <v>17</v>
@@ -1039,129 +1067,129 @@
         <v>18</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="13" t="s">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="21" t="s">
+      <c r="M6" s="14"/>
+      <c r="N6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="22" t="s">
+      <c r="O6" s="15"/>
+      <c r="P6" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="45" t="s">
+      <c r="G8" s="28"/>
+      <c r="H8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="13" t="s">
+      <c r="I8" s="29"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="13"/>
-      <c r="N8" s="21" t="s">
+      <c r="M8" s="14"/>
+      <c r="N8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="42" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
       <c r="K9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="13" t="s">
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="5"/>
       <c r="F10" s="12" t="s">
         <v>18</v>
@@ -1169,41 +1197,41 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="52" t="s">
+      <c r="J10" s="44"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="13" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="28" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="28"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="11" t="s">
         <v>32</v>
       </c>
@@ -1218,42 +1246,42 @@
       <c r="T11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="31" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="5"/>
       <c r="F13" s="11" t="s">
         <v>17</v>
@@ -1263,61 +1291,61 @@
         <v>18</v>
       </c>
       <c r="I13" s="12"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="13" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="21" t="s">
+      <c r="M13" s="14"/>
+      <c r="N13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="25" t="s">
+      <c r="O13" s="15"/>
+      <c r="P13" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="9" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="5"/>
       <c r="F15" s="11" t="s">
         <v>17</v>
@@ -1327,219 +1355,219 @@
         <v>18</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="13" t="s">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="21" t="s">
+      <c r="M15" s="14"/>
+      <c r="N15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="21"/>
-      <c r="P15" s="28" t="s">
+      <c r="O15" s="15"/>
+      <c r="P15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="13" t="s">
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="5"/>
       <c r="F17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="21" t="s">
+      <c r="I17" s="35"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="32" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="13" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="28" t="s">
+      <c r="H18" s="14"/>
+      <c r="I18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="34" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="4"/>
       <c r="F20" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="20" t="s">
+      <c r="I20" s="39"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="39" t="s">
+      <c r="M20" s="45"/>
+      <c r="N20" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="39"/>
-      <c r="P20" s="28" t="s">
+      <c r="O20" s="38"/>
+      <c r="P20" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="24" t="s">
+      <c r="D21" s="25"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="5"/>
       <c r="F22" s="11" t="s">
         <v>17</v>
@@ -1549,155 +1577,153 @@
         <v>18</v>
       </c>
       <c r="I22" s="12"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="40" t="s">
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="40"/>
-      <c r="N22" s="21" t="s">
+      <c r="M22" s="42"/>
+      <c r="N22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="28" t="s">
+      <c r="O22" s="15"/>
+      <c r="P22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="52"/>
       <c r="K23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
-      <c r="N23" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="O23" s="36"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
+      <c r="N23" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="54"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="5"/>
       <c r="F24" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="39"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="32" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="55"/>
+      <c r="T25" s="55"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="31" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="5"/>
       <c r="F27" s="11" t="s">
         <v>17</v>
@@ -1707,61 +1733,61 @@
         <v>18</v>
       </c>
       <c r="I27" s="12"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="13" t="s">
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="21" t="s">
+      <c r="M27" s="14"/>
+      <c r="N27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="21"/>
-      <c r="P27" s="22" t="s">
+      <c r="O27" s="15"/>
+      <c r="P27" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="33" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="5"/>
       <c r="F29" s="11" t="s">
         <v>17</v>
@@ -1771,65 +1797,65 @@
         <v>18</v>
       </c>
       <c r="I29" s="12"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M29" s="13"/>
-      <c r="N29" s="21" t="s">
+      <c r="M29" s="14"/>
+      <c r="N29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O29" s="21"/>
-      <c r="P29" s="28" t="s">
+      <c r="O29" s="15"/>
+      <c r="P29" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="11" t="s">
         <v>22</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="13" t="s">
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="5"/>
       <c r="F31" s="12" t="s">
         <v>30</v>
@@ -1837,49 +1863,121 @@
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="21" t="s">
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="155">
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="E5:O5"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:O7"/>
-    <mergeCell ref="K4:T4"/>
-    <mergeCell ref="P6:Q6"/>
+  <mergeCells count="150">
+    <mergeCell ref="E25:T25"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="Q31:T31"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="Q17:T17"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="E14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="N23:S23"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:O26"/>
+    <mergeCell ref="P26:T26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:O28"/>
+    <mergeCell ref="P28:T28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:T18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:O19"/>
+    <mergeCell ref="P19:T19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="P21:T21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
@@ -1904,110 +2002,33 @@
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:T18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:O19"/>
-    <mergeCell ref="P19:T19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="L24:P24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="P21:T21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:T25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:O26"/>
-    <mergeCell ref="P26:T26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="E14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="Q31:T31"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="Q17:T17"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:O7"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="E5:O5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios en jueves 3 de marzo por entrega de Laboratorio
</commit_message>
<xml_diff>
--- a/Programacion de Actividades.xlsx
+++ b/Programacion de Actividades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB45897-1960-4643-8560-2E5F6F0FC723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9492E75-F080-41AB-8AE5-FABB4495A897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="37">
   <si>
     <t>Hora</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Debo estudiar para parciales</t>
+  </si>
+  <si>
+    <t>Debo programar para cumplir con la practica 2</t>
+  </si>
+  <si>
+    <t>Seguir con P2</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,19 +427,22 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,61 +451,67 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,70 +520,67 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -853,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:O26"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,34 +892,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -970,66 +982,66 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="8"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="52"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -1041,59 +1053,59 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="31" t="s">
+      <c r="O6" s="26"/>
+      <c r="P6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="31"/>
+      <c r="Q6" s="27"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -1105,75 +1117,75 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="14"/>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="36" t="s">
+      <c r="O8" s="26"/>
+      <c r="P8" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="37"/>
+      <c r="Q8" s="47"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="34" t="s">
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
       <c r="Q9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1182,222 +1194,222 @@
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="47" t="s">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
       <c r="T10" s="9"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="35" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="14"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="11" t="s">
+      <c r="J11" s="40"/>
+      <c r="K11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="43" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="12"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M13" s="14"/>
-      <c r="N13" s="15" t="s">
+      <c r="N13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="48" t="s">
+      <c r="O13" s="26"/>
+      <c r="P13" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="49"/>
+      <c r="Q13" s="32"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="22" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12" t="s">
+      <c r="G15" s="12"/>
+      <c r="H15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="12"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M15" s="14"/>
-      <c r="N15" s="15" t="s">
+      <c r="N15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="20" t="s">
+      <c r="O15" s="26"/>
+      <c r="P15" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="31"/>
+      <c r="Q15" s="27"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="11" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="34" t="s">
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
       <c r="Q16" s="14" t="s">
         <v>24</v>
       </c>
@@ -1406,76 +1418,76 @@
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="35"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="35" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="19"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="14"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1487,59 +1499,59 @@
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
-      <c r="P19" s="40" t="s">
+      <c r="P19" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="39" t="s">
+      <c r="G20" s="12"/>
+      <c r="H20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="45" t="s">
+      <c r="I20" s="45"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="45"/>
-      <c r="N20" s="38" t="s">
+      <c r="M20" s="22"/>
+      <c r="N20" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="38"/>
-      <c r="P20" s="20" t="s">
+      <c r="O20" s="44"/>
+      <c r="P20" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="20"/>
+      <c r="Q20" s="40"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="25"/>
+      <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1551,215 +1563,215 @@
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="41" t="s">
+      <c r="P21" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12" t="s">
+      <c r="G22" s="12"/>
+      <c r="H22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="12"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="42" t="s">
+      <c r="L22" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="42"/>
-      <c r="N22" s="15" t="s">
+      <c r="M22" s="43"/>
+      <c r="N22" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="20" t="s">
+      <c r="O22" s="26"/>
+      <c r="P22" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="31"/>
+      <c r="Q22" s="27"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="50" t="s">
+      <c r="D23" s="15"/>
+      <c r="E23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="11" t="s">
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="53" t="s">
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="54"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="34"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="50" t="s">
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="52"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="18"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="35" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="55" t="s">
+      <c r="D25" s="8"/>
+      <c r="E25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="55"/>
-      <c r="S25" s="55"/>
-      <c r="T25" s="55"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="43" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="25"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12" t="s">
+      <c r="G27" s="12"/>
+      <c r="H27" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="12"/>
+      <c r="I27" s="13"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M27" s="14"/>
-      <c r="N27" s="15" t="s">
+      <c r="N27" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="15"/>
-      <c r="P27" s="31" t="s">
+      <c r="O27" s="26"/>
+      <c r="P27" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" s="31"/>
+      <c r="Q27" s="27"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="25"/>
+      <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -1771,75 +1783,77 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
-      <c r="P28" s="21" t="s">
+      <c r="P28" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="27"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="18"/>
       <c r="L29" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M29" s="14"/>
-      <c r="N29" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="O29" s="15"/>
-      <c r="P29" s="20" t="s">
+      <c r="N29" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="O29" s="57"/>
+      <c r="P29" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="27"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="34" t="s">
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
       <c r="Q30" s="14" t="s">
         <v>24</v>
       </c>
@@ -1848,37 +1862,162 @@
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
       <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="150">
+  <mergeCells count="149">
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="E5:O5"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:O7"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:T11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:O12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P7:T7"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:T18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:O19"/>
+    <mergeCell ref="P19:T19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="P21:T21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:O26"/>
+    <mergeCell ref="P26:T26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:O28"/>
+    <mergeCell ref="P28:T28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="E14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="N23:S23"/>
+    <mergeCell ref="J24:P24"/>
     <mergeCell ref="E25:T25"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="R20:T20"/>
@@ -1903,132 +2042,6 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="K23:M23"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="E14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="N23:S23"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:O26"/>
-    <mergeCell ref="P26:T26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:T18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:O19"/>
-    <mergeCell ref="P19:T19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="P21:T21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:T11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:O12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P7:T7"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:O7"/>
-    <mergeCell ref="K4:T4"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="E5:O5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Semana del 19 al 25 de marzo
</commit_message>
<xml_diff>
--- a/Programacion de Actividades.xlsx
+++ b/Programacion de Actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9492E75-F080-41AB-8AE5-FABB4495A897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A0E714-2758-4913-A1F8-B76421A30DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="46">
   <si>
     <t>Hora</t>
   </si>
@@ -136,6 +136,33 @@
   </si>
   <si>
     <t>Seguir con P2</t>
+  </si>
+  <si>
+    <t>19 al 25</t>
+  </si>
+  <si>
+    <t>Domingo 19</t>
+  </si>
+  <si>
+    <t>Lunes       20</t>
+  </si>
+  <si>
+    <t>Martes     21</t>
+  </si>
+  <si>
+    <t>Miércoles22</t>
+  </si>
+  <si>
+    <t>Jueves     23</t>
+  </si>
+  <si>
+    <t>Sábado    25</t>
+  </si>
+  <si>
+    <t>Viernes    24</t>
+  </si>
+  <si>
+    <t>Programar todo el día (Práctica 3)</t>
   </si>
 </sst>
 </file>
@@ -416,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,91 +454,82 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,67 +538,88 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -863,15 +902,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:J30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36:T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
@@ -892,34 +931,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -982,66 +1021,66 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="52"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7"/>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -1053,59 +1092,59 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="39" t="s">
+      <c r="P5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7"/>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="10"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
       <c r="L6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="26" t="s">
+      <c r="N6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="26"/>
-      <c r="P6" s="27" t="s">
+      <c r="O6" s="15"/>
+      <c r="P6" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="31"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8"/>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="25"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -1117,75 +1156,75 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="15"/>
+      <c r="C8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="26"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49" t="s">
+      <c r="G8" s="28"/>
+      <c r="H8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="49"/>
+      <c r="I8" s="29"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="20"/>
+      <c r="K8" s="24"/>
       <c r="L8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="14"/>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="46" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="47"/>
+      <c r="Q8" s="37"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="11"/>
+      <c r="C9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="27"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="38" t="s">
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
       <c r="Q9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1194,222 +1233,222 @@
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="25" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
       <c r="T10" s="9"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="14"/>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="40"/>
-      <c r="K11" s="12" t="s">
+      <c r="J11" s="20"/>
+      <c r="K11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="10" t="s">
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="8"/>
+      <c r="C13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="25"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M13" s="14"/>
-      <c r="N13" s="26" t="s">
+      <c r="N13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="26"/>
-      <c r="P13" s="31" t="s">
+      <c r="O13" s="15"/>
+      <c r="P13" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="32"/>
+      <c r="Q13" s="53"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="29" t="s">
+      <c r="C14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="7"/>
+      <c r="C15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="10"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13" t="s">
+      <c r="G15" s="11"/>
+      <c r="H15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="13"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M15" s="14"/>
-      <c r="N15" s="26" t="s">
+      <c r="N15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="26"/>
-      <c r="P15" s="40" t="s">
+      <c r="O15" s="15"/>
+      <c r="P15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="27"/>
+      <c r="Q15" s="31"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="15"/>
+      <c r="C16" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="26"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="12" t="s">
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="38" t="s">
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
       <c r="Q16" s="14" t="s">
         <v>24</v>
       </c>
@@ -1418,76 +1457,76 @@
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="42"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="35"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="L17" s="26" t="s">
+      <c r="L17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="32" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="37"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="14"/>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="7"/>
+      <c r="C19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="10"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1499,59 +1538,59 @@
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
-      <c r="P19" s="41" t="s">
+      <c r="P19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="7"/>
+      <c r="C20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="10"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="45" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="45"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="22" t="s">
+      <c r="I20" s="39"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="22"/>
-      <c r="N20" s="44" t="s">
+      <c r="M20" s="49"/>
+      <c r="N20" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="44"/>
-      <c r="P20" s="40" t="s">
+      <c r="O20" s="38"/>
+      <c r="P20" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q20" s="40"/>
+      <c r="Q20" s="20"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="8"/>
+      <c r="C21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="25"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1563,215 +1602,215 @@
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="30" t="s">
+      <c r="P21" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="11"/>
+      <c r="C22" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="27"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="13"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="43" t="s">
+      <c r="L22" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="43"/>
-      <c r="N22" s="26" t="s">
+      <c r="M22" s="42"/>
+      <c r="N22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="26"/>
-      <c r="P22" s="40" t="s">
+      <c r="O22" s="15"/>
+      <c r="P22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="27"/>
+      <c r="Q22" s="31"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="26"/>
+      <c r="E23" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="12" t="s">
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="33" t="s">
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="34"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="56"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="16" t="s">
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="18"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="47"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="32" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="10" t="s">
+      <c r="C26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="8"/>
+      <c r="C27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="25"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13" t="s">
+      <c r="G27" s="11"/>
+      <c r="H27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="13"/>
+      <c r="I27" s="12"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M27" s="14"/>
-      <c r="N27" s="26" t="s">
+      <c r="N27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="26"/>
-      <c r="P27" s="27" t="s">
+      <c r="O27" s="15"/>
+      <c r="P27" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" s="27"/>
+      <c r="Q27" s="31"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="8"/>
+      <c r="C28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="25"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -1783,77 +1822,77 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
-      <c r="P28" s="39" t="s">
+      <c r="P28" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="11"/>
+      <c r="C29" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="27"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="16" t="s">
+      <c r="G29" s="11"/>
+      <c r="H29" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="18"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="47"/>
       <c r="L29" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M29" s="14"/>
-      <c r="N29" s="57" t="s">
+      <c r="N29" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="O29" s="57"/>
-      <c r="P29" s="40" t="s">
+      <c r="O29" s="44"/>
+      <c r="P29" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="6" t="s">
+      <c r="Q29" s="20"/>
+      <c r="R29" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="11"/>
+      <c r="C30" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="27"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="12" t="s">
+      <c r="K30" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="38" t="s">
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
       <c r="Q30" s="14" t="s">
         <v>24</v>
       </c>
@@ -1862,64 +1901,387 @@
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
-      <c r="L31" s="26" t="s">
+      <c r="L31" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
       <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
     </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="12"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="14"/>
+      <c r="N34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O34" s="15"/>
+      <c r="P34" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="25"/>
+      <c r="E35" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+      <c r="B36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="14"/>
+      <c r="N36" s="61"/>
+      <c r="O36" s="61"/>
+      <c r="P36" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="59"/>
+      <c r="T36" s="59"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
+      <c r="B37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="O37" s="34"/>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
+      <c r="B38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="149">
-    <mergeCell ref="C3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="E5:O5"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:O7"/>
-    <mergeCell ref="K4:T4"/>
-    <mergeCell ref="P6:Q6"/>
+  <mergeCells count="183">
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:P38"/>
+    <mergeCell ref="Q38:T38"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:T32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:O33"/>
+    <mergeCell ref="P33:T33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:O35"/>
+    <mergeCell ref="P35:T35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="R36:T36"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="Q31:T31"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="Q17:T17"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="E14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:O26"/>
+    <mergeCell ref="P26:T26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:O28"/>
+    <mergeCell ref="P28:T28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="E25:T25"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:T18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:O19"/>
+    <mergeCell ref="P19:T19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:O21"/>
+    <mergeCell ref="P21:T21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="N23:S23"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
@@ -1944,104 +2306,33 @@
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:T18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:O19"/>
-    <mergeCell ref="P19:T19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:O21"/>
-    <mergeCell ref="P21:T21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:O26"/>
-    <mergeCell ref="P26:T26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="E14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="N23:S23"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="E25:T25"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="Q31:T31"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="Q17:T17"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:O7"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="C3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="E5:O5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>